<commit_message>
Plotting the overall sentiments
</commit_message>
<xml_diff>
--- a/data/ManUtd Matches.xlsx
+++ b/data/ManUtd Matches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anish\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anishajauhari/Desktop/UIUC/Sem 2/Data Science in Humanities/Project/SportsSentimentAnalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F86393AD-A12C-4CA6-91A3-B49289A95260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B27367-DF1E-2E49-99C8-478013C2A386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{D698C250-DC4F-47BA-9688-7B915045B274}"/>
+    <workbookView xWindow="5220" yWindow="500" windowWidth="23260" windowHeight="12720" xr2:uid="{D698C250-DC4F-47BA-9688-7B915045B274}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>Opponent</t>
   </si>
@@ -136,6 +136,18 @@
   </si>
   <si>
     <t>0-2</t>
+  </si>
+  <si>
+    <t>Watford</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>2-0</t>
+  </si>
+  <si>
+    <t>Chelsea</t>
   </si>
 </sst>
 </file>
@@ -143,7 +155,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -178,7 +190,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -494,21 +506,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D574BE2-CB6B-4F99-9837-B389F1D5388A}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -522,7 +534,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -536,7 +548,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -550,7 +562,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -564,7 +576,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -578,7 +590,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -592,7 +604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -606,7 +618,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -620,7 +632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -634,7 +646,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -648,7 +660,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -662,7 +674,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -676,7 +688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -690,7 +702,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -704,7 +716,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -718,7 +730,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -732,7 +744,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -744,6 +756,48 @@
       </c>
       <c r="D17" s="2" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1">
+        <v>44520</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="1">
+        <v>44523</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="1">
+        <v>44528</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>